<commit_message>
Update Vorlage Datenbank für v2.0.xlsx
</commit_message>
<xml_diff>
--- a/Vorlage Datenbank für v2.0.xlsx
+++ b/Vorlage Datenbank für v2.0.xlsx
@@ -459,12 +459,6 @@
     <t>res10_unit</t>
   </si>
   <si>
-    <t>img_name</t>
-  </si>
-  <si>
-    <t>img_data</t>
-  </si>
-  <si>
     <t>test_time</t>
   </si>
   <si>
@@ -832,6 +826,12 @@
   </si>
   <si>
     <t>question_author</t>
+  </si>
+  <si>
+    <t>description_img_name_1</t>
+  </si>
+  <si>
+    <t>description_img_data_1</t>
   </si>
 </sst>
 </file>
@@ -1262,8 +1262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GH19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="FO1" workbookViewId="0">
-      <selection activeCell="GH9" sqref="GH9"/>
+    <sheetView tabSelected="1" topLeftCell="EC1" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1714,159 +1714,159 @@
         <v>145</v>
       </c>
       <c r="EQ1" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="ER1" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="ES1" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="ER1" s="1" t="s">
+      <c r="ET1" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="ES1" s="1" t="s">
+      <c r="EU1" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="ET1" s="1" t="s">
+      <c r="EV1" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="EU1" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="EV1" s="1" t="s">
-        <v>151</v>
-      </c>
       <c r="EW1" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="EX1" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="EY1" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="EX1" s="1" t="s">
+      <c r="EZ1" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="EY1" s="1" t="s">
+      <c r="FA1" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="EZ1" s="1" t="s">
+      <c r="FB1" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="FA1" s="1" t="s">
+      <c r="FC1" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="FB1" s="1" t="s">
+      <c r="FD1" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="FC1" s="1" t="s">
+      <c r="FE1" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="FD1" s="1" t="s">
+      <c r="FF1" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="FE1" s="1" t="s">
+      <c r="FG1" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="FF1" s="1" t="s">
+      <c r="FH1" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="FG1" s="1" t="s">
+      <c r="FI1" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="FH1" s="1" t="s">
+      <c r="FJ1" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="FI1" s="1" t="s">
+      <c r="FK1" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="FJ1" s="1" t="s">
+      <c r="FL1" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="FK1" s="1" t="s">
+      <c r="FM1" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="FL1" s="1" t="s">
+      <c r="FN1" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="FM1" s="1" t="s">
+      <c r="FO1" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="FN1" s="1" t="s">
+      <c r="FP1" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="FO1" s="1" t="s">
+      <c r="FQ1" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="FP1" s="1" t="s">
+      <c r="FR1" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="FQ1" s="1" t="s">
+      <c r="FS1" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="FR1" s="1" t="s">
+      <c r="FT1" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="FS1" s="1" t="s">
+      <c r="FU1" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="FT1" s="1" t="s">
+      <c r="FV1" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="FU1" s="1" t="s">
+      <c r="FW1" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="FV1" s="1" t="s">
+      <c r="FX1" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="FW1" s="1" t="s">
+      <c r="FY1" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="FX1" s="1" t="s">
+      <c r="FZ1" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="FY1" s="1" t="s">
+      <c r="GA1" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="FZ1" s="1" t="s">
+      <c r="GB1" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="GA1" s="1" t="s">
+      <c r="GC1" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="GB1" s="1" t="s">
+      <c r="GD1" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="GC1" s="1" t="s">
+      <c r="GE1" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="GD1" s="1" t="s">
+      <c r="GF1" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="GE1" s="1" t="s">
+      <c r="GG1" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="GF1" s="1" t="s">
+      <c r="GH1" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="GG1" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="GH1" s="1" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="2" spans="1:190" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>154</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>232</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -1878,7 +1878,7 @@
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="R2" s="2">
         <v>15</v>
@@ -1894,7 +1894,7 @@
       </c>
       <c r="V2" s="2"/>
       <c r="W2" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="X2" s="2">
         <v>0.5</v>
@@ -1910,7 +1910,7 @@
       </c>
       <c r="AB2" s="2"/>
       <c r="AC2" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="AD2" s="2">
         <v>10</v>
@@ -1955,7 +1955,7 @@
       <c r="BJ2" s="2"/>
       <c r="BK2" s="2"/>
       <c r="BL2" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="BM2" s="2"/>
       <c r="BN2" s="2"/>
@@ -1963,7 +1963,7 @@
       <c r="BP2" s="2"/>
       <c r="BQ2" s="2"/>
       <c r="BR2" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="BS2" s="2"/>
       <c r="BT2" s="2"/>
@@ -1971,10 +1971,10 @@
       <c r="BV2" s="2"/>
       <c r="BW2" s="2"/>
       <c r="BX2" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="BY2" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="BZ2" s="2">
         <v>0</v>
@@ -2013,7 +2013,7 @@
       <c r="CX2" s="2"/>
       <c r="CY2" s="2"/>
       <c r="CZ2" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="DA2" s="2"/>
       <c r="DB2" s="2"/>
@@ -2022,7 +2022,7 @@
       <c r="DE2" s="2"/>
       <c r="DF2" s="2"/>
       <c r="DG2" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="DH2" s="2"/>
       <c r="DI2" s="2"/>
@@ -2031,7 +2031,7 @@
       <c r="DL2" s="2"/>
       <c r="DM2" s="2"/>
       <c r="DN2" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="DO2" s="2"/>
       <c r="DP2" s="2"/>
@@ -2040,7 +2040,7 @@
       <c r="DS2" s="2"/>
       <c r="DT2" s="2"/>
       <c r="DU2" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="DV2" s="2"/>
       <c r="DW2" s="2"/>
@@ -2049,7 +2049,7 @@
       <c r="DZ2" s="2"/>
       <c r="EA2" s="2"/>
       <c r="EB2" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="EC2" s="2"/>
       <c r="ED2" s="2"/>
@@ -2058,7 +2058,7 @@
       <c r="EG2" s="2"/>
       <c r="EH2" s="2"/>
       <c r="EI2" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="EJ2" s="2"/>
       <c r="EK2" s="2"/>
@@ -2067,41 +2067,41 @@
       <c r="EN2" s="2"/>
       <c r="EO2" s="2"/>
       <c r="EP2" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="EQ2" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="EQ2" s="2" t="s">
-        <v>160</v>
-      </c>
       <c r="ES2" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="ET2" s="2"/>
       <c r="EU2" s="2"/>
       <c r="EV2" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:190" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>154</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>232</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -2113,7 +2113,7 @@
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="R3" s="2">
         <v>0.1</v>
@@ -2129,7 +2129,7 @@
       </c>
       <c r="V3" s="2"/>
       <c r="W3" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="X3" s="2">
         <v>0.1</v>
@@ -2193,7 +2193,7 @@
       <c r="BW3" s="2"/>
       <c r="BX3" s="2"/>
       <c r="BY3" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="BZ3" s="2">
         <v>0</v>
@@ -2275,41 +2275,41 @@
       <c r="EO3" s="2"/>
       <c r="EP3" s="2"/>
       <c r="EQ3" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="ER3" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="ES3" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="ET3" s="2"/>
       <c r="EU3" s="2"/>
       <c r="EV3" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:190" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>154</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>232</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -2321,7 +2321,7 @@
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="R4" s="2">
         <v>10</v>
@@ -2337,7 +2337,7 @@
       </c>
       <c r="V4" s="2"/>
       <c r="W4" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="X4" s="2">
         <v>2</v>
@@ -2353,7 +2353,7 @@
       </c>
       <c r="AB4" s="2"/>
       <c r="AC4" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="AD4" s="2">
         <v>20</v>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="AH4" s="2"/>
       <c r="AI4" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="AJ4" s="2">
         <v>100</v>
@@ -2421,7 +2421,7 @@
       <c r="BW4" s="2"/>
       <c r="BX4" s="2"/>
       <c r="BY4" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="BZ4" s="2">
         <v>-20000000</v>
@@ -2503,41 +2503,41 @@
       <c r="EO4" s="2"/>
       <c r="EP4" s="2"/>
       <c r="EQ4" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="ER4" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="ES4" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="ET4" s="2"/>
       <c r="EU4" s="2"/>
       <c r="EV4" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:190" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>154</v>
-      </c>
       <c r="D5" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E5" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>232</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -2549,7 +2549,7 @@
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="R5" s="2">
         <v>1</v>
@@ -2565,7 +2565,7 @@
       </c>
       <c r="V5" s="2"/>
       <c r="W5" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="X5" s="2">
         <v>0.1</v>
@@ -2629,7 +2629,7 @@
       <c r="BW5" s="2"/>
       <c r="BX5" s="2"/>
       <c r="BY5" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="BZ5" s="2">
         <v>-20000000</v>
@@ -2711,41 +2711,41 @@
       <c r="EO5" s="2"/>
       <c r="EP5" s="2"/>
       <c r="EQ5" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="ER5" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="ES5" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="ET5" s="2"/>
       <c r="EU5" s="2"/>
       <c r="EV5" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:190" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>154</v>
-      </c>
       <c r="D6" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E6" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>232</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -2757,7 +2757,7 @@
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="R6" s="2">
         <v>1</v>
@@ -2773,7 +2773,7 @@
       </c>
       <c r="V6" s="2"/>
       <c r="W6" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="X6" s="2">
         <v>2</v>
@@ -2789,7 +2789,7 @@
       </c>
       <c r="AB6" s="2"/>
       <c r="AC6" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="AD6" s="2">
         <v>30</v>
@@ -2847,7 +2847,7 @@
       <c r="BW6" s="2"/>
       <c r="BX6" s="2"/>
       <c r="BY6" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="BZ6" s="2">
         <v>0</v>
@@ -2929,41 +2929,41 @@
       <c r="EO6" s="2"/>
       <c r="EP6" s="2"/>
       <c r="EQ6" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="ER6" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="ES6" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="ET6" s="2"/>
       <c r="EU6" s="2"/>
       <c r="EV6" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:190" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>154</v>
-      </c>
       <c r="D7" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E7" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>232</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -2975,7 +2975,7 @@
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
       <c r="Q7" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="R7" s="2">
         <v>1</v>
@@ -2991,7 +2991,7 @@
       </c>
       <c r="V7" s="2"/>
       <c r="W7" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="X7" s="2">
         <v>1000</v>
@@ -3055,7 +3055,7 @@
       <c r="BW7" s="2"/>
       <c r="BX7" s="2"/>
       <c r="BY7" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="BZ7" s="2">
         <v>-1000000</v>
@@ -3137,41 +3137,41 @@
       <c r="EO7" s="2"/>
       <c r="EP7" s="2"/>
       <c r="EQ7" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="ER7" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="ES7" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="ET7" s="2"/>
       <c r="EU7" s="2"/>
       <c r="EV7" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:190" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>154</v>
-      </c>
       <c r="D8" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E8" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>232</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -3183,7 +3183,7 @@
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="R8" s="2">
         <v>100</v>
@@ -3199,7 +3199,7 @@
       </c>
       <c r="V8" s="2"/>
       <c r="W8" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="X8" s="2">
         <v>1</v>
@@ -3215,7 +3215,7 @@
       </c>
       <c r="AB8" s="2"/>
       <c r="AC8" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="AD8" s="2">
         <v>1</v>
@@ -3231,7 +3231,7 @@
       </c>
       <c r="AH8" s="2"/>
       <c r="AI8" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="AJ8" s="2">
         <v>10</v>
@@ -3283,7 +3283,7 @@
       <c r="BW8" s="2"/>
       <c r="BX8" s="2"/>
       <c r="BY8" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="BZ8" s="2">
         <v>-100000</v>
@@ -3365,41 +3365,41 @@
       <c r="EO8" s="2"/>
       <c r="EP8" s="2"/>
       <c r="EQ8" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="ER8" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="ES8" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="ET8" s="2"/>
       <c r="EU8" s="2"/>
       <c r="EV8" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" spans="1:190" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>154</v>
-      </c>
       <c r="D9" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E9" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>232</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -3411,7 +3411,7 @@
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="R9" s="2">
         <v>100</v>
@@ -3427,7 +3427,7 @@
       </c>
       <c r="V9" s="2"/>
       <c r="W9" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="X9" s="2">
         <v>1</v>
@@ -3443,7 +3443,7 @@
       </c>
       <c r="AB9" s="2"/>
       <c r="AC9" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="AD9" s="2">
         <v>1</v>
@@ -3459,7 +3459,7 @@
       </c>
       <c r="AH9" s="2"/>
       <c r="AI9" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="AJ9" s="2">
         <v>10</v>
@@ -3511,7 +3511,7 @@
       <c r="BW9" s="2"/>
       <c r="BX9" s="2"/>
       <c r="BY9" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="BZ9" s="2">
         <v>-100000</v>
@@ -3593,41 +3593,41 @@
       <c r="EO9" s="2"/>
       <c r="EP9" s="2"/>
       <c r="EQ9" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="ER9" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="ES9" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="ET9" s="2"/>
       <c r="EU9" s="2"/>
       <c r="EV9" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="10" spans="1:190" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>154</v>
-      </c>
       <c r="D10" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E10" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>232</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -3639,7 +3639,7 @@
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="R10" s="2">
         <v>10</v>
@@ -3655,7 +3655,7 @@
       </c>
       <c r="V10" s="2"/>
       <c r="W10" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="X10" s="2">
         <v>10</v>
@@ -3671,7 +3671,7 @@
       </c>
       <c r="AB10" s="2"/>
       <c r="AC10" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="AD10" s="2">
         <v>10</v>
@@ -3729,7 +3729,7 @@
       <c r="BW10" s="2"/>
       <c r="BX10" s="2"/>
       <c r="BY10" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="BZ10" s="2">
         <v>-100000</v>
@@ -3811,41 +3811,41 @@
       <c r="EO10" s="2"/>
       <c r="EP10" s="2"/>
       <c r="EQ10" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="ER10" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="ES10" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="ET10" s="2"/>
       <c r="EU10" s="2"/>
       <c r="EV10" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="11" spans="1:190" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>154</v>
-      </c>
       <c r="D11" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E11" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>232</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -3857,7 +3857,7 @@
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
       <c r="Q11" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="R11" s="2">
         <v>10</v>
@@ -3873,7 +3873,7 @@
       </c>
       <c r="V11" s="2"/>
       <c r="W11" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="X11" s="2">
         <v>0.1</v>
@@ -3889,7 +3889,7 @@
       </c>
       <c r="AB11" s="2"/>
       <c r="AC11" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="AD11" s="2">
         <v>1</v>
@@ -3947,7 +3947,7 @@
       <c r="BW11" s="2"/>
       <c r="BX11" s="2"/>
       <c r="BY11" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="BZ11" s="2">
         <v>-10000</v>
@@ -4029,41 +4029,41 @@
       <c r="EO11" s="2"/>
       <c r="EP11" s="2"/>
       <c r="EQ11" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="ER11" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="ES11" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="ET11" s="2"/>
       <c r="EU11" s="2"/>
       <c r="EV11" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="12" spans="1:190" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>154</v>
-      </c>
       <c r="D12" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E12" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>232</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -4075,7 +4075,7 @@
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
       <c r="Q12" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="R12" s="2">
         <v>10</v>
@@ -4091,7 +4091,7 @@
       </c>
       <c r="V12" s="2"/>
       <c r="W12" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="X12" s="2">
         <v>1</v>
@@ -4155,7 +4155,7 @@
       <c r="BW12" s="2"/>
       <c r="BX12" s="2"/>
       <c r="BY12" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="BZ12" s="2">
         <v>-10000</v>
@@ -4237,41 +4237,41 @@
       <c r="EO12" s="2"/>
       <c r="EP12" s="2"/>
       <c r="EQ12" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="ER12" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="ES12" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="ET12" s="2"/>
       <c r="EU12" s="2"/>
       <c r="EV12" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:190" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>154</v>
-      </c>
       <c r="D13" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E13" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>232</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -4283,7 +4283,7 @@
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="R13" s="2">
         <v>10</v>
@@ -4299,7 +4299,7 @@
       </c>
       <c r="V13" s="2"/>
       <c r="W13" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="X13" s="2">
         <v>50</v>
@@ -4363,7 +4363,7 @@
       <c r="BW13" s="2"/>
       <c r="BX13" s="2"/>
       <c r="BY13" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="BZ13" s="2">
         <v>-10000</v>
@@ -4445,41 +4445,41 @@
       <c r="EO13" s="2"/>
       <c r="EP13" s="2"/>
       <c r="EQ13" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="ER13" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="ES13" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="ET13" s="2"/>
       <c r="EU13" s="2"/>
       <c r="EV13" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="14" spans="1:190" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>154</v>
-      </c>
       <c r="D14" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E14" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>232</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -4491,7 +4491,7 @@
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="R14" s="2">
         <v>1.2</v>
@@ -4507,7 +4507,7 @@
       </c>
       <c r="V14" s="2"/>
       <c r="W14" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="X14" s="2">
         <v>5</v>
@@ -4523,7 +4523,7 @@
       </c>
       <c r="AB14" s="2"/>
       <c r="AC14" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="AD14" s="2">
         <v>1</v>
@@ -4581,7 +4581,7 @@
       <c r="BW14" s="2"/>
       <c r="BX14" s="2"/>
       <c r="BY14" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="BZ14" s="2">
         <v>0</v>
@@ -4663,41 +4663,41 @@
       <c r="EO14" s="2"/>
       <c r="EP14" s="2"/>
       <c r="EQ14" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="ER14" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="ES14" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="ET14" s="2"/>
       <c r="EU14" s="2"/>
       <c r="EV14" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="15" spans="1:190" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>154</v>
-      </c>
       <c r="D15" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E15" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>232</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -4709,7 +4709,7 @@
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="R15" s="2">
         <v>20</v>
@@ -4725,7 +4725,7 @@
       </c>
       <c r="V15" s="2"/>
       <c r="W15" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="X15" s="2">
         <v>1</v>
@@ -4741,7 +4741,7 @@
       </c>
       <c r="AB15" s="2"/>
       <c r="AC15" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="AD15" s="2">
         <v>2</v>
@@ -4757,7 +4757,7 @@
       </c>
       <c r="AH15" s="2"/>
       <c r="AI15" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AJ15" s="2">
         <v>10</v>
@@ -4809,7 +4809,7 @@
       <c r="BW15" s="2"/>
       <c r="BX15" s="2"/>
       <c r="BY15" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="BZ15" s="2">
         <v>0</v>
@@ -4891,41 +4891,41 @@
       <c r="EO15" s="2"/>
       <c r="EP15" s="2"/>
       <c r="EQ15" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="ER15" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="ES15" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="ET15" s="2"/>
       <c r="EU15" s="2"/>
       <c r="EV15" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="16" spans="1:190" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>154</v>
-      </c>
       <c r="D16" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E16" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>232</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -4937,7 +4937,7 @@
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
       <c r="Q16" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="R16" s="2">
         <v>1</v>
@@ -4953,7 +4953,7 @@
       </c>
       <c r="V16" s="2"/>
       <c r="W16" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="X16" s="2">
         <v>1</v>
@@ -5017,7 +5017,7 @@
       <c r="BW16" s="2"/>
       <c r="BX16" s="2"/>
       <c r="BY16" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="BZ16" s="2">
         <v>0</v>
@@ -5099,41 +5099,41 @@
       <c r="EO16" s="2"/>
       <c r="EP16" s="2"/>
       <c r="EQ16" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="ER16" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="ES16" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="ET16" s="2"/>
       <c r="EU16" s="2"/>
       <c r="EV16" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="17" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>154</v>
-      </c>
       <c r="D17" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E17" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>232</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -5145,7 +5145,7 @@
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
       <c r="Q17" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="R17" s="2">
         <v>1</v>
@@ -5161,7 +5161,7 @@
       </c>
       <c r="V17" s="2"/>
       <c r="W17" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="X17" s="2">
         <v>1</v>
@@ -5177,7 +5177,7 @@
       </c>
       <c r="AB17" s="2"/>
       <c r="AC17" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="AD17" s="2">
         <v>1</v>
@@ -5235,7 +5235,7 @@
       <c r="BW17" s="2"/>
       <c r="BX17" s="2"/>
       <c r="BY17" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="BZ17" s="2">
         <v>0</v>
@@ -5317,41 +5317,41 @@
       <c r="EO17" s="2"/>
       <c r="EP17" s="2"/>
       <c r="EQ17" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="ER17" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="ES17" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="ET17" s="2"/>
       <c r="EU17" s="2"/>
       <c r="EV17" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="18" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>154</v>
-      </c>
       <c r="D18" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E18" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>232</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
@@ -5363,7 +5363,7 @@
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
       <c r="Q18" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="R18" s="2">
         <v>0.05</v>
@@ -5379,7 +5379,7 @@
       </c>
       <c r="V18" s="2"/>
       <c r="W18" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="X18" s="2">
         <v>5</v>
@@ -5443,7 +5443,7 @@
       <c r="BW18" s="2"/>
       <c r="BX18" s="2"/>
       <c r="BY18" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="BZ18" s="2">
         <v>0</v>
@@ -5525,41 +5525,41 @@
       <c r="EO18" s="2"/>
       <c r="EP18" s="2"/>
       <c r="EQ18" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="ER18" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="ES18" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="ET18" s="2"/>
       <c r="EU18" s="2"/>
       <c r="EV18" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="19" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>154</v>
-      </c>
       <c r="D19" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E19" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>232</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -5571,7 +5571,7 @@
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="R19" s="2">
         <v>100</v>
@@ -5587,7 +5587,7 @@
       </c>
       <c r="V19" s="2"/>
       <c r="W19" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="X19" s="2">
         <v>0.1</v>
@@ -5651,7 +5651,7 @@
       <c r="BW19" s="2"/>
       <c r="BX19" s="2"/>
       <c r="BY19" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="BZ19" s="2">
         <v>-10000</v>
@@ -5733,18 +5733,18 @@
       <c r="EO19" s="2"/>
       <c r="EP19" s="2"/>
       <c r="EQ19" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="ER19" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="ES19" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="ET19" s="2"/>
       <c r="EU19" s="2"/>
       <c r="EV19" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>